<commit_message>
Updated test data and manual cases to include multiple categories
</commit_message>
<xml_diff>
--- a/manual/Manual_Test_Cases.xlsx
+++ b/manual/Manual_Test_Cases.xlsx
@@ -472,15 +472,16 @@
         <v>TC_003</v>
       </c>
       <c r="B4" t="str">
-        <v>Verify Cart Subtotal Calculation</v>
+        <v>Verify Cart Subtotal Calculation with Multiple Categories</v>
       </c>
       <c r="C4" t="str" xml:space="preserve">
-        <v xml:space="preserve">1. Add 'Computing and Internet' ($10) to cart
-2. Add 'Fiction' ($24) to cart
-3. Navigate to Shopping Cart</v>
+        <v xml:space="preserve">1. Add 'Computing and Internet' (Books) to cart
+2. Add 'Blue Jeans' (Apparel &amp; Shoes) to cart
+3. Add 'Black &amp; White Diamond Heart' (Jewelry) to cart
+4. Navigate to Shopping Cart</v>
       </c>
       <c r="D4" t="str">
-        <v>Cart shows 2 items. Subtotal displays exactly $34.00.</v>
+        <v>Cart shows 3 items from different categories. Subtotal displays exactly $141.00 (10 + 1 + 130).</v>
       </c>
       <c r="E4" t="str">
         <v>High</v>

</xml_diff>